<commit_message>
DZ01 v1 initial upload
</commit_message>
<xml_diff>
--- a/docs/DZ01/NeighbourConnect-StudijaIzvedivosti.xlsx
+++ b/docs/DZ01/NeighbourConnect-StudijaIzvedivosti.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\Private\FER\Semestar8\Kolegiji\infsus\projekt\NeighbourConnect\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\Private\FER\Semestar8\Kolegiji\infsus\projekt\NeighbourConnect\docs\DZ01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D91E4B-D4AB-45BF-A7A5-EB5963AF694A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2534641-B5EA-4C1A-86A6-1C3362E81FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Karakteristike</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Vremenski najpovoljnije rješenje jer kupujemo gotov proizvod. Međutim, ekonomski je vrlo nepovoljno rješenje s obzirom da plaćamo niz usluga. Također, dobiveno rješenje može sadržavati puno više funkcionalnosti nego što je potrebno za normalan rad našeg sustava.</t>
+  </si>
+  <si>
+    <t>Komentar alternative</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -747,17 +750,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -790,46 +782,98 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -841,7 +885,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -849,12 +893,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -870,18 +908,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,18 +921,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,16 +929,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -926,18 +940,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -963,12 +965,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -986,65 +982,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1054,18 +1011,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1075,43 +1020,229 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1421,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EEE08C-145C-49B9-A7B2-D920AF3FF34A}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:S5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,706 +1562,788 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="135" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="135" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="35" t="s">
         <v>13</v>
       </c>
+      <c r="K1" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="74"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="61" t="s">
+      <c r="A2" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6">
-        <v>2</v>
-      </c>
-      <c r="G2" s="6">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6">
-        <v>3</v>
-      </c>
-      <c r="I2" s="6">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3">
-        <v>3</v>
-      </c>
-      <c r="K2" s="103" t="s">
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="J2" s="64">
+        <v>3</v>
+      </c>
+      <c r="K2" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="101"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
-      <c r="B3" s="62" t="s">
+      <c r="A3" s="92"/>
+      <c r="B3" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7">
-        <v>3</v>
-      </c>
-      <c r="H3" s="7">
-        <v>2</v>
-      </c>
-      <c r="I3" s="7">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4">
-        <v>3</v>
-      </c>
-      <c r="K3" s="103"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2</v>
+      </c>
+      <c r="J3" s="65">
+        <v>3</v>
+      </c>
+      <c r="K3" s="102"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
       <c r="S3" s="104"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="62" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="37" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
-        <v>2</v>
-      </c>
-      <c r="F4" s="7">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7">
-        <v>2</v>
-      </c>
-      <c r="H4" s="7">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7">
-        <v>3</v>
-      </c>
-      <c r="J4" s="4">
-        <v>2</v>
-      </c>
-      <c r="K4" s="103"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3</v>
+      </c>
+      <c r="J4" s="65">
+        <v>2</v>
+      </c>
+      <c r="K4" s="102"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103"/>
+      <c r="R4" s="103"/>
       <c r="S4" s="104"/>
     </row>
     <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="63" t="s">
+      <c r="A5" s="93"/>
+      <c r="B5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2</v>
-      </c>
-      <c r="F5" s="9">
-        <v>3</v>
-      </c>
-      <c r="G5" s="9">
-        <v>3</v>
-      </c>
-      <c r="H5" s="9">
-        <v>3</v>
-      </c>
-      <c r="I5" s="9">
-        <v>3</v>
-      </c>
-      <c r="J5" s="10">
-        <v>3</v>
-      </c>
-      <c r="K5" s="103"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7">
+        <v>3</v>
+      </c>
+      <c r="J5" s="66">
+        <v>3</v>
+      </c>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="107"/>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="14">
+      <c r="B6" s="90"/>
+      <c r="C6" s="10">
         <f>AVERAGE(C2:C5)</f>
         <v>2.5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <f t="shared" ref="D6:J6" si="0">AVERAGE(D2:D5)</f>
         <v>2.5</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="67">
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="N6" s="1"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="77"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11">
-        <v>2</v>
-      </c>
-      <c r="D7" s="12">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12">
-        <v>2</v>
-      </c>
-      <c r="F7" s="12">
-        <v>2</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12">
-        <v>2</v>
-      </c>
-      <c r="I7" s="12">
-        <v>2</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2</v>
+      </c>
+      <c r="J7" s="68">
         <v>1</v>
       </c>
-      <c r="K7" s="105" t="s">
+      <c r="K7" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="110"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
-      <c r="B8" s="62" t="s">
+      <c r="A8" s="92"/>
+      <c r="B8" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="G8" s="7">
-        <v>2</v>
-      </c>
-      <c r="H8" s="7">
-        <v>3</v>
-      </c>
-      <c r="I8" s="7">
-        <v>2</v>
-      </c>
-      <c r="J8" s="4">
-        <v>2</v>
-      </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
+      <c r="G8" s="5">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2</v>
+      </c>
+      <c r="J8" s="65">
+        <v>2</v>
+      </c>
+      <c r="K8" s="111"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="112"/>
+      <c r="O8" s="112"/>
+      <c r="P8" s="112"/>
+      <c r="Q8" s="112"/>
+      <c r="R8" s="112"/>
+      <c r="S8" s="113"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
-      <c r="B9" s="62" t="s">
+      <c r="A9" s="92"/>
+      <c r="B9" s="37" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="7">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="7">
-        <v>2</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2</v>
-      </c>
-      <c r="H9" s="7">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7">
-        <v>2</v>
-      </c>
-      <c r="J9" s="4">
-        <v>2</v>
-      </c>
-      <c r="K9" s="105"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2</v>
+      </c>
+      <c r="J9" s="65">
+        <v>2</v>
+      </c>
+      <c r="K9" s="111"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="112"/>
+      <c r="O9" s="112"/>
+      <c r="P9" s="112"/>
+      <c r="Q9" s="112"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="113"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="66"/>
-      <c r="B10" s="63" t="s">
+      <c r="A10" s="93"/>
+      <c r="B10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8">
-        <v>2</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>2</v>
-      </c>
-      <c r="F10" s="9">
-        <v>2</v>
-      </c>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9">
-        <v>3</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2</v>
-      </c>
-      <c r="J10" s="10">
-        <v>2</v>
-      </c>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
+      <c r="J10" s="66">
+        <v>2</v>
+      </c>
+      <c r="K10" s="114"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="115"/>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="115"/>
+      <c r="R10" s="115"/>
+      <c r="S10" s="116"/>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="14">
+      <c r="B11" s="90"/>
+      <c r="C11" s="10">
         <f>AVERAGE(C7:C10)</f>
         <v>2</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="10">
         <f t="shared" ref="D11:J11" si="1">AVERAGE(D7:D10)</f>
         <v>1.75</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="10">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="10">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J11" s="41">
+      <c r="J11" s="67">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
+      <c r="K11" s="75"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="76"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="77"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="61" t="s">
+      <c r="A12" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11">
-        <v>3</v>
-      </c>
-      <c r="D12" s="12">
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="12">
-        <v>3</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G12" s="12">
-        <v>2</v>
-      </c>
-      <c r="H12" s="12">
-        <v>2</v>
-      </c>
-      <c r="I12" s="12">
-        <v>2</v>
-      </c>
-      <c r="J12" s="13">
+      <c r="G12" s="9">
+        <v>2</v>
+      </c>
+      <c r="H12" s="9">
+        <v>2</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2</v>
+      </c>
+      <c r="J12" s="68">
         <v>1</v>
       </c>
-      <c r="K12" s="105" t="s">
+      <c r="K12" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="110"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
-      <c r="B13" s="62" t="s">
+      <c r="A13" s="92"/>
+      <c r="B13" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="7">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7">
-        <v>3</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2</v>
-      </c>
-      <c r="G13" s="7">
-        <v>2</v>
-      </c>
-      <c r="H13" s="7">
-        <v>3</v>
-      </c>
-      <c r="I13" s="7">
-        <v>2</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3</v>
+      </c>
+      <c r="I13" s="5">
+        <v>2</v>
+      </c>
+      <c r="J13" s="65">
         <v>1</v>
       </c>
-      <c r="K13" s="105"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="113"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
-      <c r="B14" s="62" t="s">
+      <c r="A14" s="92"/>
+      <c r="B14" s="37" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="7">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>3</v>
-      </c>
-      <c r="F14" s="7">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7">
-        <v>3</v>
-      </c>
-      <c r="H14" s="7">
-        <v>2</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>3</v>
+      </c>
+      <c r="H14" s="5">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5">
         <v>1</v>
       </c>
-      <c r="J14" s="4">
-        <v>3</v>
-      </c>
-      <c r="K14" s="105"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="106"/>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="106"/>
-      <c r="R14" s="106"/>
-      <c r="S14" s="106"/>
+      <c r="J14" s="65">
+        <v>3</v>
+      </c>
+      <c r="K14" s="111"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="112"/>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="113"/>
     </row>
     <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="66"/>
-      <c r="B15" s="63" t="s">
+      <c r="A15" s="93"/>
+      <c r="B15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>1</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="9">
-        <v>3</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="9">
-        <v>2</v>
-      </c>
-      <c r="H15" s="9">
+      <c r="G15" s="7">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7">
         <v>1</v>
       </c>
-      <c r="I15" s="9">
-        <v>2</v>
-      </c>
-      <c r="J15" s="10">
+      <c r="I15" s="7">
+        <v>2</v>
+      </c>
+      <c r="J15" s="66">
         <v>1</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
-      <c r="O15" s="106"/>
-      <c r="P15" s="106"/>
-      <c r="Q15" s="106"/>
-      <c r="R15" s="106"/>
-      <c r="S15" s="106"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
+      <c r="N15" s="115"/>
+      <c r="O15" s="115"/>
+      <c r="P15" s="115"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="115"/>
+      <c r="S15" s="116"/>
     </row>
     <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="14">
+      <c r="B16" s="95"/>
+      <c r="C16" s="10">
         <f>AVERAGE(C12:C15)</f>
         <v>2.5</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="10">
         <f t="shared" ref="D16:J16" si="2">AVERAGE(D12:D15)</f>
         <v>1.75</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="10">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="10">
         <f t="shared" si="2"/>
         <v>1.75</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="10">
         <f t="shared" si="2"/>
         <v>2.25</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="10">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="10">
         <f t="shared" si="2"/>
         <v>1.75</v>
       </c>
-      <c r="J16" s="41">
+      <c r="J16" s="67">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="56"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="57"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="67" t="s">
+      <c r="K16" s="78"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="79"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="80"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="97"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="83"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="46" t="s">
+      <c r="B18" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="33"/>
+      <c r="F18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="58" t="s">
+      <c r="J18" s="69" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
-      <c r="B19" s="69" t="s">
+      <c r="K18" s="81"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="83"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="92"/>
+      <c r="B19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="59"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="66"/>
-      <c r="B20" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="45" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="83"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="93"/>
+      <c r="B20" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="16" t="s">
+      <c r="D20" s="32"/>
+      <c r="E20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="60"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="85"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K6:S6"/>
+    <mergeCell ref="K11:S11"/>
+    <mergeCell ref="K16:S20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A7:A10"/>
@@ -2138,11 +2351,6 @@
     <mergeCell ref="K2:S5"/>
     <mergeCell ref="K7:S10"/>
     <mergeCell ref="K12:S15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2163,249 +2371,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="83">
+      <c r="B1" s="50">
         <v>275000</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="86">
+      <c r="A2" s="53">
         <v>0.05</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="43">
         <v>0</v>
       </c>
-      <c r="C2" s="73">
+      <c r="C2" s="44">
         <f>B2+1</f>
         <v>1</v>
       </c>
-      <c r="D2" s="73">
+      <c r="D2" s="44">
         <f>C2+1</f>
         <v>2</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="54" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="71">
+      <c r="B3" s="42">
         <f>ROUNDUP(12*2*1100/57%,-3)</f>
         <v>47000</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="42">
         <f>B3</f>
         <v>47000</v>
       </c>
-      <c r="D3" s="71">
+      <c r="D3" s="42">
         <f t="shared" ref="D3:D7" si="0">C3</f>
         <v>47000</v>
       </c>
-      <c r="E3" s="89"/>
+      <c r="E3" s="117"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="71">
+      <c r="B4" s="42">
         <f>ROUNDUP(12*2*800/75%,-3)</f>
         <v>26000</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="42">
         <f t="shared" ref="C4" si="1">B4</f>
         <v>26000</v>
       </c>
-      <c r="D4" s="71">
+      <c r="D4" s="42">
         <f t="shared" si="0"/>
         <v>26000</v>
       </c>
-      <c r="E4" s="90"/>
+      <c r="E4" s="118"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="71">
+      <c r="B5" s="42">
         <f>B11*12%</f>
         <v>6600</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="42">
         <f>C11*12%</f>
         <v>9900</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="42">
         <f>D11*12%</f>
         <v>16500</v>
       </c>
-      <c r="E5" s="90"/>
+      <c r="E5" s="118"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="42">
         <v>10000</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="42">
         <v>0</v>
       </c>
-      <c r="D6" s="71">
+      <c r="D6" s="42">
         <v>0</v>
       </c>
-      <c r="E6" s="90"/>
+      <c r="E6" s="118"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="42">
         <f>B6*17.5%</f>
         <v>1750</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="42">
         <f t="shared" ref="C7" si="2">B7</f>
         <v>1750</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="42">
         <f t="shared" si="0"/>
         <v>1750</v>
       </c>
-      <c r="E7" s="92"/>
+      <c r="E7" s="119"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="74">
+      <c r="B8" s="45">
         <f>SUM(B3:B7)</f>
         <v>91350</v>
       </c>
-      <c r="C8" s="74">
+      <c r="C8" s="45">
         <f>SUM(C3:C7)</f>
         <v>84650</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="45">
         <f>SUM(D3:D7)</f>
         <v>91250</v>
       </c>
-      <c r="E8" s="93">
+      <c r="E8" s="57">
         <f>B8+NPV(A$2,C8:D8)</f>
         <v>254735.48752834465</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="94"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="89"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="117"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="75">
+      <c r="B10" s="46">
         <v>0.2</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="46">
         <v>0.3</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="46">
         <v>0.5</v>
       </c>
-      <c r="E10" s="92"/>
+      <c r="E10" s="119"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="47">
         <f>Budžet*B10</f>
         <v>55000</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="47">
         <f>Budžet*C10</f>
         <v>82500</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D11" s="47">
         <f>Budžet*D10</f>
         <v>137500</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="57">
         <f>B11+NPV(A$2,C11:D11)</f>
         <v>258287.98185941041</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="96"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="97"/>
+      <c r="A12" s="124"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="59"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="77">
+      <c r="B13" s="48">
         <f>B11-B8</f>
         <v>-36350</v>
       </c>
-      <c r="C13" s="77">
+      <c r="C13" s="48">
         <f>C11-C8</f>
         <v>-2150</v>
       </c>
-      <c r="D13" s="77">
+      <c r="D13" s="48">
         <f>D11-D8</f>
         <v>46250</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="60">
         <f>B13+NPV(A$2,C13:D13)</f>
         <v>3552.4943310657545</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="48">
         <f>B13/POWER(1+$A$2,B2)</f>
         <v>-36350</v>
       </c>
-      <c r="C14" s="77">
+      <c r="C14" s="48">
         <f>C13/POWER(1+$A$2,C2)</f>
         <v>-2047.6190476190475</v>
       </c>
-      <c r="D14" s="77">
+      <c r="D14" s="48">
         <f>D13/POWER(1+$A$2,D2)</f>
         <v>41950.113378684808</v>
       </c>
-      <c r="E14" s="89"/>
+      <c r="E14" s="117"/>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="100">
+      <c r="B15" s="62">
         <f>B14</f>
         <v>-36350</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="62">
         <f>B15+C14</f>
         <v>-38397.619047619046</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="62">
         <f>C15+D14</f>
         <v>3552.4943310657618</v>
       </c>
-      <c r="E15" s="101"/>
+      <c r="E15" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2424,7 +2632,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2434,299 +2642,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="31"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="134"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33" t="s">
+      <c r="A2" s="130"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="27">
-        <v>3</v>
-      </c>
-      <c r="C3" s="28">
+      <c r="B3" s="17">
+        <v>3</v>
+      </c>
+      <c r="C3" s="18">
         <v>5</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="18">
         <f>B3*C3</f>
         <v>15</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="18">
         <v>4</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="18">
         <f>E3*B3</f>
         <v>12</v>
       </c>
-      <c r="G3" s="28">
-        <v>2</v>
-      </c>
-      <c r="H3" s="35">
+      <c r="G3" s="18">
+        <v>2</v>
+      </c>
+      <c r="H3" s="21">
         <f>G3*B3</f>
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="13">
         <v>0</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="13">
         <f t="shared" ref="D4:D10" si="0">B4*C4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="13">
         <v>5</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="13">
         <f t="shared" ref="F4:F10" si="1">E4*B4</f>
         <v>5</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="13">
         <v>0</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="22">
         <f t="shared" ref="H4:H10" si="2">G4*B4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22">
-        <v>3</v>
-      </c>
-      <c r="C5" s="21">
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E5" s="21">
-        <v>3</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="13">
         <v>5</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="22">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="21">
-        <v>3</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="C6" s="13">
+        <v>3</v>
+      </c>
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="13">
+        <v>2</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13">
         <v>4</v>
       </c>
-      <c r="F6" s="21">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="G6" s="21">
-        <v>2</v>
-      </c>
-      <c r="H6" s="36">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="22">
-        <v>2</v>
-      </c>
-      <c r="C7" s="21">
-        <v>4</v>
-      </c>
-      <c r="D7" s="21">
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E7" s="21">
-        <v>3</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="E7" s="13">
+        <v>3</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="13">
         <v>5</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="22">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="14">
         <v>1</v>
       </c>
-      <c r="C8" s="21">
-        <v>3</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E8" s="21">
-        <v>3</v>
-      </c>
-      <c r="F8" s="21">
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G8" s="21">
-        <v>3</v>
-      </c>
-      <c r="H8" s="36">
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="22">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22">
-        <v>2</v>
-      </c>
-      <c r="C9" s="21">
-        <v>3</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E9" s="21">
-        <v>3</v>
-      </c>
-      <c r="F9" s="21">
+      <c r="E9" s="13">
+        <v>3</v>
+      </c>
+      <c r="F9" s="13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="13">
         <v>5</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="22">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="38">
-        <v>2</v>
-      </c>
-      <c r="C10" s="39">
+      <c r="B10" s="24">
+        <v>2</v>
+      </c>
+      <c r="C10" s="25">
         <v>5</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="25">
         <v>4</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="25">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="25">
         <v>0</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43">
+      <c r="B11" s="28"/>
+      <c r="C11" s="127">
         <f>SUM(D3:D10)</f>
         <v>57</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43">
+      <c r="D11" s="127"/>
+      <c r="E11" s="127">
         <f>SUM(F3:F10)</f>
-        <v>53</v>
-      </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43">
+        <v>52</v>
+      </c>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127">
         <f>SUM(H3:H10)</f>
         <v>46</v>
       </c>
-      <c r="H11" s="44"/>
+      <c r="H11" s="128"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>

</xml_diff>